<commit_message>
Add annotation files and update datasets
Added multiple annotation guides, sample files, and reference CSVs for NHAMCS coding. Updated and reorganized MIMIC tabular data, including new annotation samples and moved/removed legacy and intermediate files to streamline the dataset structure.
</commit_message>
<xml_diff>
--- a/Annotation/Annot_test_icd_MIMIC_hypercap.xlsx
+++ b/Annotation/Annot_test_icd_MIMIC_hypercap.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reblocke/Research/Hypercap-CC-NLP/Annotation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blocke/Box Sync/Residency Personal Files/Scholarly Work/Locke Research Projects/Hypercap-CC-NLP/Annotation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D77994-39EE-4148-B1B5-CE1432B47F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B1598A-E137-D843-8DA0-13A5B86A4015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="2000" windowWidth="26180" windowHeight="24680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="700" windowWidth="33980" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hypercap_cohort" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="113">
   <si>
     <t>subject_id</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>Uncodable/Unknown</t>
+  </si>
+  <si>
+    <t>Chest pain</t>
+  </si>
+  <si>
+    <t>Altered mental status</t>
   </si>
 </sst>
 </file>
@@ -363,9 +369,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="169" formatCode="&quot;General&quot;;&quot;Psychological&quot;;&quot;Nervous system&quot;;&quot;Eye &amp; Ear&quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot;General&quot;;&quot;Psychological&quot;;&quot;Nervous system&quot;;&quot;Eye &amp; Ear&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,6 +394,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -451,13 +463,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -470,10 +482,11 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BV10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AT2" sqref="AT2"/>
+    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="BN11" sqref="BN11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1112,6 +1125,18 @@
       <c r="AO2" s="2">
         <v>96413.618749999994</v>
       </c>
+      <c r="BM2" t="s">
+        <v>111</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>96</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>57</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="3" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -1198,6 +1223,18 @@
       <c r="AI3" s="2">
         <v>103125.32708333329</v>
       </c>
+      <c r="BM3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="BN3" t="s">
+        <v>97</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>53</v>
+      </c>
+      <c r="BP3" s="10" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="4" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -1296,6 +1333,12 @@
       <c r="AO4" s="2">
         <v>83154.656944444447</v>
       </c>
+      <c r="BM4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="5" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -1376,6 +1419,12 @@
       <c r="Z5">
         <v>98.3</v>
       </c>
+      <c r="BM5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="BN5" s="10" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="6" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -1444,6 +1493,12 @@
       <c r="AI6" s="2">
         <v>89078.273611111115</v>
       </c>
+      <c r="BM6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="BN6" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="7" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -1542,6 +1597,12 @@
       <c r="AF7" s="2">
         <v>94893.998611111107</v>
       </c>
+      <c r="BM7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="BN7" s="10" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="8" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -1622,6 +1683,12 @@
       <c r="Z8">
         <v>97.7</v>
       </c>
+      <c r="BM8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="BN8" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="9" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -1684,6 +1751,9 @@
       <c r="T9">
         <v>2</v>
       </c>
+      <c r="BM9" s="7" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="10" spans="1:74" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -1763,6 +1833,12 @@
       </c>
       <c r="Z10">
         <v>98.2</v>
+      </c>
+      <c r="BM10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="BN10" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1774,7 +1850,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13752379-98CE-764A-B04D-62B3179E6059}">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>